<commit_message>
Limit rows shown by default
</commit_message>
<xml_diff>
--- a/students.xlsx
+++ b/students.xlsx
@@ -13,7 +13,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <si>
-    <t>Student</t>
+    <t>Name</t>
   </si>
   <si>
     <t>Age</t>
@@ -44,25 +44,95 @@
   </si>
   <si>
     <t>Harry</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Kerry</t>
+  </si>
+  <si>
+    <t>Lars</t>
+  </si>
+  <si>
+    <t>Monty</t>
+  </si>
+  <si>
+    <t>Nick</t>
+  </si>
+  <si>
+    <t>Ophelia</t>
+  </si>
+  <si>
+    <t>Peter</t>
+  </si>
+  <si>
+    <t>Quentin</t>
+  </si>
+  <si>
+    <t>Rebecca</t>
+  </si>
+  <si>
+    <t>Sarah</t>
+  </si>
+  <si>
+    <t>Tamara</t>
+  </si>
+  <si>
+    <t>Ulysses</t>
+  </si>
+  <si>
+    <t>Veronica</t>
+  </si>
+  <si>
+    <t>William</t>
+  </si>
+  <si>
+    <t>Xavier</t>
+  </si>
+  <si>
+    <t>Yvonne</t>
+  </si>
+  <si>
+    <t>Zander</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF222222"/>
+    </font>
     <font/>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF9F9F9"/>
+        <bgColor rgb="FFF9F9F9"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -83,9 +153,15 @@
   <cellStyleXfs count="1">
     <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
-    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="1">
+    <xf applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="1" applyFill="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf applyAlignment="1" fillId="3" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="1" applyFill="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="2">
       <alignment/>
     </xf>
   </cellXfs>
@@ -104,7 +180,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane topLeftCell="A2" ySplit="1.0" activePane="bottomLeft" state="frozen"/>
+      <selection sqref="B3" activeCell="B3" pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
@@ -131,13 +210,13 @@
       </c>
     </row>
     <row r="3">
-      <c t="s" s="1" r="A3">
+      <c t="s" s="2" r="A3">
         <v>4</v>
       </c>
-      <c s="1" r="B3">
+      <c s="2" r="B3">
         <v>13.0</v>
       </c>
-      <c s="1" r="C3">
+      <c s="2" r="C3">
         <v>5.0</v>
       </c>
     </row>
@@ -153,13 +232,13 @@
       </c>
     </row>
     <row r="5">
-      <c t="s" s="1" r="A5">
+      <c t="s" s="2" r="A5">
         <v>6</v>
       </c>
-      <c s="1" r="B5">
-        <v>12.0</v>
-      </c>
-      <c s="1" r="C5">
+      <c s="2" r="B5">
+        <v>12.0</v>
+      </c>
+      <c s="2" r="C5">
         <v>5.0</v>
       </c>
     </row>
@@ -175,13 +254,13 @@
       </c>
     </row>
     <row r="7">
-      <c t="s" s="1" r="A7">
+      <c t="s" s="2" r="A7">
         <v>8</v>
       </c>
-      <c s="1" r="B7">
-        <v>12.0</v>
-      </c>
-      <c s="1" r="C7">
+      <c s="2" r="B7">
+        <v>12.0</v>
+      </c>
+      <c s="2" r="C7">
         <v>3.0</v>
       </c>
     </row>
@@ -197,15 +276,225 @@
       </c>
     </row>
     <row r="9">
-      <c t="s" s="1" r="A9">
+      <c t="s" s="2" r="A9">
         <v>10</v>
       </c>
-      <c s="1" r="B9">
+      <c s="2" r="B9">
         <v>16.0</v>
       </c>
-      <c s="1" r="C9">
-        <v>5.0</v>
-      </c>
+      <c s="2" r="C9">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c t="s" s="3" r="A10">
+        <v>11</v>
+      </c>
+      <c s="3" r="B10">
+        <v>12.0</v>
+      </c>
+      <c s="1" r="C10">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c t="s" s="3" r="A11">
+        <v>12</v>
+      </c>
+      <c s="3" r="B11">
+        <v>13.0</v>
+      </c>
+      <c s="2" r="C11">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c t="s" s="3" r="A12">
+        <v>13</v>
+      </c>
+      <c s="3" r="B12">
+        <v>14.0</v>
+      </c>
+      <c s="1" r="C12">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c t="s" s="3" r="A13">
+        <v>14</v>
+      </c>
+      <c s="3" r="B13">
+        <v>15.0</v>
+      </c>
+      <c s="2" r="C13">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c t="s" s="3" r="A14">
+        <v>15</v>
+      </c>
+      <c s="3" r="B14">
+        <v>14.0</v>
+      </c>
+      <c s="1" r="C14">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c t="s" s="3" r="A15">
+        <v>16</v>
+      </c>
+      <c s="3" r="B15">
+        <v>14.0</v>
+      </c>
+      <c s="2" r="C15">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c t="s" s="3" r="A16">
+        <v>17</v>
+      </c>
+      <c s="3" r="B16">
+        <v>14.0</v>
+      </c>
+      <c s="1" r="C16">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c t="s" s="3" r="A17">
+        <v>18</v>
+      </c>
+      <c s="3" r="B17">
+        <v>14.0</v>
+      </c>
+      <c s="2" r="C17">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c t="s" s="3" r="A18">
+        <v>19</v>
+      </c>
+      <c s="3" r="B18">
+        <v>13.0</v>
+      </c>
+      <c s="1" r="C18">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c t="s" s="3" r="A19">
+        <v>20</v>
+      </c>
+      <c s="3" r="B19">
+        <v>12.0</v>
+      </c>
+      <c s="2" r="C19">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c t="s" s="3" r="A20">
+        <v>21</v>
+      </c>
+      <c s="3" r="B20">
+        <v>14.0</v>
+      </c>
+      <c s="1" r="C20">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c t="s" s="3" r="A21">
+        <v>22</v>
+      </c>
+      <c s="3" r="B21">
+        <v>15.0</v>
+      </c>
+      <c s="2" r="C21">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c t="s" s="3" r="A22">
+        <v>23</v>
+      </c>
+      <c s="3" r="B22">
+        <v>14.0</v>
+      </c>
+      <c s="1" r="C22">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c t="s" s="3" r="A23">
+        <v>24</v>
+      </c>
+      <c s="3" r="B23">
+        <v>14.0</v>
+      </c>
+      <c s="2" r="C23">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c t="s" s="3" r="A24">
+        <v>25</v>
+      </c>
+      <c s="3" r="B24">
+        <v>12.0</v>
+      </c>
+      <c s="1" r="C24">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c t="s" s="3" r="A25">
+        <v>26</v>
+      </c>
+      <c s="3" r="B25">
+        <v>12.0</v>
+      </c>
+      <c s="2" r="C25">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c t="s" s="3" r="A26">
+        <v>27</v>
+      </c>
+      <c s="3" r="B26">
+        <v>14.0</v>
+      </c>
+      <c s="1" r="C26">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c t="s" s="3" r="A27">
+        <v>28</v>
+      </c>
+      <c s="3" r="B27">
+        <v>14.0</v>
+      </c>
+      <c s="2" r="C27">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c s="3" r="B28"/>
+      <c s="1" r="C28"/>
+    </row>
+    <row r="29">
+      <c s="3" r="B29"/>
+      <c s="2" r="C29"/>
+    </row>
+    <row r="30">
+      <c s="3" r="B30"/>
+      <c s="1" r="C30"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>